<commit_message>
Update to ATT&CK v11
</commit_message>
<xml_diff>
--- a/data/dettect_data_sources.xlsx
+++ b/data/dettect_data_sources.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/VSCode/DeTTECT-private/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/VSCode-DeTTECT-prod/DeTTECT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FA5988-B1A8-1340-896E-46E865AC3DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E53A19-8430-484E-A673-0921F901B1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="27700" windowHeight="17500" xr2:uid="{CA121E54-A6AA-1848-A706-0DCFA18BBC16}"/>
+    <workbookView xWindow="34560" yWindow="-12540" windowWidth="51200" windowHeight="28300" xr2:uid="{CA121E54-A6AA-1848-A706-0DCFA18BBC16}"/>
   </bookViews>
   <sheets>
     <sheet name="Techniques" sheetId="4" r:id="rId1"/>
     <sheet name="DeTT&amp;CT data sources" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Techniques!$A$1:$H$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Techniques!$A$1:$H$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="221">
   <si>
     <t>T1612</t>
   </si>
@@ -668,6 +668,39 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>T1595.003</t>
+  </si>
+  <si>
+    <t>Wordlist Scanning</t>
+  </si>
+  <si>
+    <t>ATT&amp;CK v11 - Network Traffic Content</t>
+  </si>
+  <si>
+    <t>Email Addresses</t>
+  </si>
+  <si>
+    <t>T1557.003</t>
+  </si>
+  <si>
+    <t>DHCP Spoofing</t>
+  </si>
+  <si>
+    <t>T1589</t>
+  </si>
+  <si>
+    <t>Gather Victim Identity Information</t>
+  </si>
+  <si>
+    <t>T1033</t>
+  </si>
+  <si>
+    <t>System Owner/User Discovery</t>
+  </si>
+  <si>
+    <t>T1589.002</t>
   </si>
 </sst>
 </file>
@@ -1094,13 +1127,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1343,34 +1376,30 @@
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="H11" s="10"/>
+        <v>179</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>190</v>
@@ -1382,21 +1411,19 @@
         <v>185</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>179</v>
-      </c>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>164</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>190</v>
@@ -1408,17 +1435,21 @@
         <v>185</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+        <v>188</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>190</v>
@@ -1437,10 +1468,10 @@
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>190</v>
@@ -1452,41 +1483,43 @@
         <v>185</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>190</v>
@@ -1501,12 +1534,12 @@
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>190</v>
@@ -1515,24 +1548,18 @@
         <v>207</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>190</v>
@@ -1543,16 +1570,22 @@
       <c r="E19" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>190</v>
@@ -1561,7 +1594,7 @@
         <v>207</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -1569,10 +1602,10 @@
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>190</v>
@@ -1581,7 +1614,7 @@
         <v>207</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1589,10 +1622,10 @@
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>190</v>
@@ -1601,7 +1634,7 @@
         <v>207</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1609,10 +1642,10 @@
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>159</v>
+        <v>33</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>190</v>
@@ -1621,20 +1654,18 @@
         <v>207</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>190</v>
@@ -1643,18 +1674,20 @@
         <v>207</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F24" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>190</v>
@@ -1663,7 +1696,7 @@
         <v>207</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -1671,10 +1704,10 @@
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>190</v>
@@ -1685,18 +1718,16 @@
       <c r="E26" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>179</v>
-      </c>
+      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>190</v>
@@ -1707,16 +1738,18 @@
       <c r="E27" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F27" s="9"/>
+      <c r="F27" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>156</v>
+        <v>58</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>157</v>
+        <v>59</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>190</v>
@@ -1725,7 +1758,7 @@
         <v>207</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -1733,10 +1766,10 @@
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>190</v>
@@ -1745,7 +1778,7 @@
         <v>207</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -1753,10 +1786,10 @@
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>190</v>
@@ -1773,10 +1806,10 @@
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>190</v>
@@ -1793,10 +1826,10 @@
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>190</v>
@@ -1813,10 +1846,10 @@
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>152</v>
+        <v>66</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>153</v>
+        <v>67</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>190</v>
@@ -1825,22 +1858,18 @@
         <v>207</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>188</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>190</v>
@@ -1849,24 +1878,22 @@
         <v>207</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F34" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G34" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>179</v>
-      </c>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>190</v>
@@ -1889,10 +1916,10 @@
     </row>
     <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>190</v>
@@ -1915,10 +1942,10 @@
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>149</v>
+        <v>55</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>190</v>
@@ -1930,17 +1957,21 @@
         <v>185</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+        <v>188</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>190</v>
@@ -1951,16 +1982,18 @@
       <c r="E38" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F38" s="9"/>
+      <c r="F38" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>190</v>
@@ -1969,59 +2002,55 @@
         <v>207</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40" s="12"/>
+        <v>137</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="D40" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="F40" s="9"/>
+        <v>207</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>190</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="C41" s="12"/>
       <c r="D41" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>188</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>190</v>
@@ -2042,10 +2071,10 @@
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>147</v>
+        <v>79</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>190</v>
@@ -2054,18 +2083,22 @@
         <v>207</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>190</v>
@@ -2082,10 +2115,10 @@
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>190</v>
@@ -2102,10 +2135,10 @@
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>190</v>
@@ -2114,20 +2147,18 @@
         <v>207</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>190</v>
@@ -2136,18 +2167,20 @@
         <v>207</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F47" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>190</v>
@@ -2164,10 +2197,10 @@
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>190</v>
@@ -2184,10 +2217,10 @@
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>190</v>
@@ -2204,10 +2237,10 @@
     </row>
     <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>190</v>
@@ -2224,10 +2257,10 @@
     </row>
     <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>190</v>
@@ -2244,10 +2277,10 @@
     </row>
     <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>190</v>
@@ -2264,10 +2297,10 @@
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>190</v>
@@ -2284,10 +2317,10 @@
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>190</v>
@@ -2304,10 +2337,10 @@
     </row>
     <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>190</v>
@@ -2324,10 +2357,10 @@
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>190</v>
@@ -2344,10 +2377,10 @@
     </row>
     <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>190</v>
@@ -2356,27 +2389,27 @@
         <v>207</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>202</v>
+      <c r="A59" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -2384,10 +2417,10 @@
     </row>
     <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>198</v>
@@ -2403,14 +2436,14 @@
       <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>13</v>
+      <c r="A61" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>207</v>
@@ -2424,10 +2457,10 @@
     </row>
     <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>190</v>
@@ -2444,13 +2477,13 @@
     </row>
     <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>102</v>
+        <v>214</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>207</v>
@@ -2464,10 +2497,10 @@
     </row>
     <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>190</v>
@@ -2484,10 +2517,10 @@
     </row>
     <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>190</v>
@@ -2504,10 +2537,10 @@
     </row>
     <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>190</v>
@@ -2524,10 +2557,10 @@
     </row>
     <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>190</v>
@@ -2536,20 +2569,18 @@
         <v>207</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>186</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
     </row>
     <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>190</v>
@@ -2558,7 +2589,7 @@
         <v>207</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
@@ -2566,10 +2597,10 @@
     </row>
     <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>190</v>
@@ -2578,20 +2609,20 @@
         <v>207</v>
       </c>
       <c r="E69" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F69" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>185</v>
       </c>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
     </row>
     <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>190</v>
@@ -2600,7 +2631,7 @@
         <v>207</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
@@ -2608,10 +2639,10 @@
     </row>
     <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>190</v>
@@ -2620,18 +2651,20 @@
         <v>207</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F71" s="9"/>
+        <v>186</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
     </row>
     <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C72" s="12" t="s">
         <v>190</v>
@@ -2648,10 +2681,10 @@
     </row>
     <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C73" s="12" t="s">
         <v>190</v>
@@ -2668,10 +2701,10 @@
     </row>
     <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>190</v>
@@ -2680,42 +2713,38 @@
         <v>207</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
       <c r="H74" s="9"/>
     </row>
     <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>183</v>
+        <v>84</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C75" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="D75" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
     </row>
     <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>190</v>
@@ -2726,36 +2755,40 @@
       <c r="E76" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
+      <c r="F76" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="H76" s="9"/>
     </row>
     <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>183</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>190</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C77" s="12"/>
       <c r="D77" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F77" s="9"/>
+        <v>206</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
     </row>
     <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>190</v>
@@ -2764,22 +2797,18 @@
         <v>207</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G78" s="9" t="s">
         <v>188</v>
       </c>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
       <c r="H78" s="9"/>
     </row>
     <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>190</v>
@@ -2788,22 +2817,18 @@
         <v>207</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
       <c r="H79" s="9"/>
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>190</v>
@@ -2817,15 +2842,17 @@
       <c r="F80" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G80" s="9"/>
+      <c r="G80" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H80" s="9"/>
     </row>
     <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>190</v>
@@ -2837,17 +2864,19 @@
         <v>185</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G81" s="9"/>
+        <v>188</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="H81" s="9"/>
     </row>
     <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>190</v>
@@ -2865,51 +2894,55 @@
       <c r="H82" s="9"/>
     </row>
     <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>203</v>
+      <c r="A83" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F83" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
     </row>
     <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>199</v>
+      <c r="A84" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F84" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
     </row>
     <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>198</v>
@@ -2926,7 +2959,7 @@
     </row>
     <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>199</v>
@@ -2945,14 +2978,14 @@
       <c r="H86" s="9"/>
     </row>
     <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>25</v>
+      <c r="A87" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>207</v>
@@ -2965,14 +2998,14 @@
       <c r="H87" s="9"/>
     </row>
     <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>23</v>
+      <c r="A88" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>207</v>
@@ -2985,20 +3018,20 @@
       <c r="H88" s="9"/>
     </row>
     <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>21</v>
+      <c r="A89" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>186</v>
@@ -3007,20 +3040,20 @@
       <c r="H89" s="9"/>
     </row>
     <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>19</v>
+      <c r="A90" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
@@ -3028,10 +3061,10 @@
     </row>
     <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>190</v>
@@ -3040,7 +3073,7 @@
         <v>207</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
@@ -3048,10 +3081,10 @@
     </row>
     <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C92" s="12" t="s">
         <v>190</v>
@@ -3060,23 +3093,21 @@
         <v>207</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F92" s="9"/>
       <c r="G92" s="9"/>
       <c r="H92" s="9"/>
     </row>
     <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>11</v>
+        <v>211</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>207</v>
@@ -3090,10 +3121,10 @@
     </row>
     <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>190</v>
@@ -3102,18 +3133,20 @@
         <v>207</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F94" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
     </row>
     <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>190</v>
@@ -3122,7 +3155,7 @@
         <v>207</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="9"/>
@@ -3130,10 +3163,10 @@
     </row>
     <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>190</v>
@@ -3142,7 +3175,7 @@
         <v>207</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
@@ -3150,10 +3183,10 @@
     </row>
     <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>190</v>
@@ -3162,41 +3195,43 @@
         <v>207</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F97" s="9"/>
+        <v>186</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
     </row>
     <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
       <c r="H98" s="9"/>
     </row>
     <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>200</v>
+      <c r="A99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>207</v>
@@ -3208,14 +3243,114 @@
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
     </row>
+    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9"/>
+    </row>
+    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+    </row>
+    <row r="102" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+    </row>
+    <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+    </row>
+    <row r="104" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H99" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H99">
-      <sortCondition ref="A1:A99"/>
+  <autoFilter ref="A1:H104" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H104">
+      <sortCondition ref="A1:A104"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H93">
-    <sortCondition ref="A1:A93"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H98">
+    <sortCondition ref="A1:A98"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -3230,7 +3365,7 @@
           <x14:formula1>
             <xm:f>'DeTT&amp;CT data sources'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:F12 F13 E15:F23 G2:G23 H2:H10 H12:H23 E39 E24:H38 E40:H1048576 G39:H39</xm:sqref>
+          <xm:sqref>E2:F13 F14 E16:F24 G2:G24 H2:H11 H13:H24 E40 E25:H39 G40:H40 E41:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3281,6 +3416,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C10F0625C0942243B06F014CA94A1AFE" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2042c6bc1cae45920cbe57d817eddad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c6cd37b1-e58f-4b4d-9972-86df42eb1d84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="012bfb64603ca90dd9e4209826fe8536" ns2:_="">
     <xsd:import namespace="c6cd37b1-e58f-4b4d-9972-86df42eb1d84"/>
@@ -3470,15 +3614,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3486,6 +3621,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5DBBFA0-4896-4F89-83F2-9B6F36081FF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{606D9982-FF33-4FCF-965C-160E67E8EBF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3499,14 +3642,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5DBBFA0-4896-4F89-83F2-9B6F36081FF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
ATT&CK v12 update for DeTT&CT data sources
</commit_message>
<xml_diff>
--- a/data/dettect_data_sources.xlsx
+++ b/data/dettect_data_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mb/VSCode-DeTTECT-prod/DeTTECT/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruben/vscode-projects/vscode-prd/DeTTECT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E53A19-8430-484E-A673-0921F901B1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E223523B-8D99-4D41-97FE-3F3AF3AD579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="-12540" windowWidth="51200" windowHeight="28300" xr2:uid="{CA121E54-A6AA-1848-A706-0DCFA18BBC16}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="39880" windowHeight="25100" xr2:uid="{CA121E54-A6AA-1848-A706-0DCFA18BBC16}"/>
   </bookViews>
   <sheets>
     <sheet name="Techniques" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="234">
   <si>
     <t>T1612</t>
   </si>
@@ -701,6 +701,45 @@
   </si>
   <si>
     <t>T1589.002</t>
+  </si>
+  <si>
+    <t>T1199</t>
+  </si>
+  <si>
+    <t>T1537</t>
+  </si>
+  <si>
+    <t>T1087.002</t>
+  </si>
+  <si>
+    <t>T1482</t>
+  </si>
+  <si>
+    <t>T1039</t>
+  </si>
+  <si>
+    <t>T1133</t>
+  </si>
+  <si>
+    <t>Trusted Relationship</t>
+  </si>
+  <si>
+    <t>Transfer Data to Cloud Account</t>
+  </si>
+  <si>
+    <t>Domain Account</t>
+  </si>
+  <si>
+    <t>Domain Trust Discovery</t>
+  </si>
+  <si>
+    <t>Data from Network Shared Drive</t>
+  </si>
+  <si>
+    <t>External Remote Services</t>
+  </si>
+  <si>
+    <t>ATT&amp;CK v12 - Network Traffic Content</t>
   </si>
 </sst>
 </file>
@@ -1127,13 +1166,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B16:B17"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1395,35 +1434,28 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="A12" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>207</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="H12" s="10"/>
+        <v>179</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>190</v>
@@ -1435,21 +1467,19 @@
         <v>185</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>179</v>
-      </c>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>164</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>190</v>
@@ -1461,17 +1491,21 @@
         <v>185</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+        <v>188</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>190</v>
@@ -1490,10 +1524,10 @@
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>190</v>
@@ -1505,21 +1539,17 @@
         <v>185</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>190</v>
@@ -1528,18 +1558,24 @@
         <v>207</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>190</v>
@@ -1556,10 +1592,10 @@
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>190</v>
@@ -1568,24 +1604,18 @@
         <v>207</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>190</v>
@@ -1596,16 +1626,22 @@
       <c r="E20" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>190</v>
@@ -1614,7 +1650,7 @@
         <v>207</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -1622,10 +1658,10 @@
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>190</v>
@@ -1634,7 +1670,7 @@
         <v>207</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1642,10 +1678,10 @@
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>190</v>
@@ -1654,7 +1690,7 @@
         <v>207</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -1662,10 +1698,10 @@
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>159</v>
+        <v>33</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>190</v>
@@ -1674,40 +1710,35 @@
         <v>207</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="A25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>207</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>190</v>
@@ -1718,16 +1749,18 @@
       <c r="E26" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>190</v>
@@ -1736,20 +1769,18 @@
         <v>207</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>190</v>
@@ -1766,10 +1797,10 @@
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>190</v>
@@ -1778,18 +1809,20 @@
         <v>207</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F29" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>154</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>190</v>
@@ -1806,10 +1839,10 @@
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>157</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>190</v>
@@ -1818,7 +1851,7 @@
         <v>207</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -1826,10 +1859,10 @@
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>68</v>
+        <v>154</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>155</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>190</v>
@@ -1846,10 +1879,10 @@
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>190</v>
@@ -1866,10 +1899,10 @@
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>152</v>
+        <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>190</v>
@@ -1878,22 +1911,18 @@
         <v>207</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>188</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>150</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>151</v>
+        <v>67</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>190</v>
@@ -1904,22 +1933,16 @@
       <c r="E35" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F35" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>179</v>
-      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>56</v>
+        <v>152</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>57</v>
+        <v>153</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>190</v>
@@ -1928,24 +1951,22 @@
         <v>207</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F36" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>179</v>
-      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>55</v>
+        <v>151</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>190</v>
@@ -1968,10 +1989,10 @@
     </row>
     <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>190</v>
@@ -1983,17 +2004,21 @@
         <v>185</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+        <v>188</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>190</v>
@@ -2004,53 +2029,64 @@
       <c r="E39" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="F39" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="A40" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>207</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="F40" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C41" s="12"/>
+        <v>149</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="D41" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="F41" s="9"/>
+        <v>207</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>190</v>
@@ -2061,20 +2097,16 @@
       <c r="E42" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>188</v>
-      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
       <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>190</v>
@@ -2083,27 +2115,22 @@
         <v>207</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>188</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="G43" s="9"/>
       <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="A44" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>207</v>
       </c>
       <c r="E44" s="9" t="s">
@@ -2115,19 +2142,17 @@
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>190</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="C45" s="12"/>
       <c r="D45" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>179</v>
+        <v>206</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -2135,10 +2160,10 @@
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>190</v>
@@ -2147,18 +2172,22 @@
         <v>207</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>141</v>
+        <v>79</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>190</v>
@@ -2170,17 +2199,19 @@
         <v>185</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G47" s="9"/>
+        <v>186</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>190</v>
@@ -2197,10 +2228,10 @@
     </row>
     <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>190</v>
@@ -2217,10 +2248,10 @@
     </row>
     <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>190</v>
@@ -2237,10 +2268,10 @@
     </row>
     <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>190</v>
@@ -2249,18 +2280,20 @@
         <v>207</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F51" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>190</v>
@@ -2276,31 +2309,28 @@
       <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="A53" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>207</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>190</v>
@@ -2317,10 +2347,10 @@
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>190</v>
@@ -2337,10 +2367,10 @@
     </row>
     <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>190</v>
@@ -2357,10 +2387,10 @@
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>190</v>
@@ -2377,10 +2407,10 @@
     </row>
     <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>190</v>
@@ -2397,10 +2427,10 @@
     </row>
     <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>190</v>
@@ -2409,21 +2439,21 @@
         <v>207</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>202</v>
+      <c r="A60" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>207</v>
@@ -2436,14 +2466,14 @@
       <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>201</v>
+      <c r="A61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>207</v>
@@ -2457,10 +2487,10 @@
     </row>
     <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>190</v>
@@ -2477,13 +2507,13 @@
     </row>
     <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>214</v>
+        <v>122</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>215</v>
+        <v>123</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>207</v>
@@ -2497,10 +2527,10 @@
     </row>
     <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>190</v>
@@ -2509,41 +2539,38 @@
         <v>207</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
     </row>
     <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D65" s="4" t="s">
+      <c r="A65" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>207</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
     </row>
     <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>101</v>
+      <c r="A66" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>207</v>
@@ -2556,14 +2583,14 @@
       <c r="H66" s="9"/>
     </row>
     <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>99</v>
+      <c r="A67" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>207</v>
@@ -2577,10 +2604,10 @@
     </row>
     <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>190</v>
@@ -2597,32 +2624,30 @@
     </row>
     <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>94</v>
+        <v>214</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>95</v>
+        <v>215</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>186</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
     </row>
     <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>190</v>
@@ -2631,7 +2656,7 @@
         <v>207</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
@@ -2639,10 +2664,10 @@
     </row>
     <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>190</v>
@@ -2651,20 +2676,18 @@
         <v>207</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
     </row>
     <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C72" s="12" t="s">
         <v>190</v>
@@ -2673,7 +2696,7 @@
         <v>207</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
@@ -2681,10 +2704,10 @@
     </row>
     <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C73" s="12" t="s">
         <v>190</v>
@@ -2693,7 +2716,7 @@
         <v>207</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
@@ -2701,10 +2724,10 @@
     </row>
     <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>190</v>
@@ -2713,7 +2736,7 @@
         <v>207</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
@@ -2721,10 +2744,10 @@
     </row>
     <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>190</v>
@@ -2735,16 +2758,18 @@
       <c r="E75" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F75" s="9"/>
+      <c r="F75" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
     </row>
     <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>190</v>
@@ -2753,29 +2778,27 @@
         <v>207</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
       <c r="H76" s="9"/>
     </row>
     <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>183</v>
+        <v>92</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C77" s="12"/>
+        <v>15</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>190</v>
+      </c>
       <c r="D77" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>188</v>
+        <v>207</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>185</v>
@@ -2785,10 +2808,10 @@
     </row>
     <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>190</v>
@@ -2797,7 +2820,7 @@
         <v>207</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
@@ -2805,10 +2828,10 @@
     </row>
     <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>190</v>
@@ -2817,7 +2840,7 @@
         <v>207</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
@@ -2825,10 +2848,10 @@
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>190</v>
@@ -2839,20 +2862,16 @@
       <c r="E80" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F80" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G80" s="9" t="s">
-        <v>188</v>
-      </c>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
       <c r="H80" s="9"/>
     </row>
     <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>190</v>
@@ -2863,20 +2882,16 @@
       <c r="E81" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F81" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>179</v>
-      </c>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
     <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>190</v>
@@ -2885,42 +2900,42 @@
         <v>207</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G82" s="9"/>
+      <c r="G82" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="H82" s="9"/>
     </row>
     <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>190</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C83" s="12"/>
       <c r="D83" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>185</v>
+        <v>206</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
     </row>
     <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>190</v>
@@ -2929,23 +2944,21 @@
         <v>207</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
     </row>
     <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>203</v>
+      <c r="A85" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>207</v>
@@ -2958,116 +2971,128 @@
       <c r="H85" s="9"/>
     </row>
     <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>199</v>
+      <c r="A86" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="H86" s="9"/>
     </row>
     <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>204</v>
+      <c r="A87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="H87" s="9"/>
     </row>
     <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>199</v>
+      <c r="A88" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F88" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
     </row>
     <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>217</v>
+      <c r="A89" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
     </row>
     <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>213</v>
+      <c r="A90" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F90" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
     </row>
     <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>25</v>
+      <c r="A91" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>207</v>
@@ -3080,14 +3105,14 @@
       <c r="H91" s="9"/>
     </row>
     <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>23</v>
+      <c r="A92" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>207</v>
@@ -3100,14 +3125,14 @@
       <c r="H92" s="9"/>
     </row>
     <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>211</v>
+      <c r="A93" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>207</v>
@@ -3120,62 +3145,62 @@
       <c r="H93" s="9"/>
     </row>
     <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>21</v>
+      <c r="A94" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>186</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F94" s="9"/>
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
     </row>
     <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>19</v>
+      <c r="A95" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F95" s="9"/>
+        <v>179</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="G95" s="9"/>
       <c r="H95" s="9"/>
     </row>
     <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>17</v>
+      <c r="A96" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
@@ -3183,10 +3208,10 @@
     </row>
     <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>190</v>
@@ -3195,20 +3220,18 @@
         <v>207</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="F97" s="9"/>
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
     </row>
     <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>190</v>
@@ -3225,13 +3248,13 @@
     </row>
     <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>207</v>
@@ -3245,10 +3268,10 @@
     </row>
     <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>190</v>
@@ -3257,18 +3280,20 @@
         <v>207</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F100" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>186</v>
+      </c>
       <c r="G100" s="9"/>
       <c r="H100" s="9"/>
     </row>
     <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>190</v>
@@ -3277,7 +3302,7 @@
         <v>207</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F101" s="9"/>
       <c r="G101" s="9"/>
@@ -3285,10 +3310,10 @@
     </row>
     <row r="102" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>190</v>
@@ -3297,7 +3322,7 @@
         <v>207</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
@@ -3305,33 +3330,35 @@
     </row>
     <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>207</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F103" s="9"/>
+        <v>186</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="G103" s="9"/>
       <c r="H103" s="9"/>
     </row>
     <row r="104" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>200</v>
+      <c r="A104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>207</v>
@@ -3343,10 +3370,130 @@
       <c r="G104" s="9"/>
       <c r="H104" s="9"/>
     </row>
+    <row r="105" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+    </row>
+    <row r="106" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+    </row>
+    <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+    </row>
+    <row r="108" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+    </row>
+    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F109" s="9"/>
+      <c r="G109" s="9"/>
+      <c r="H109" s="9"/>
+    </row>
+    <row r="110" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H104" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H104">
-      <sortCondition ref="A1:A104"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H110">
+      <sortCondition ref="A1:A110"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H98">
@@ -3416,15 +3563,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C10F0625C0942243B06F014CA94A1AFE" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2042c6bc1cae45920cbe57d817eddad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c6cd37b1-e58f-4b4d-9972-86df42eb1d84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="012bfb64603ca90dd9e4209826fe8536" ns2:_="">
     <xsd:import namespace="c6cd37b1-e58f-4b4d-9972-86df42eb1d84"/>
@@ -3614,6 +3752,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3621,14 +3768,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5DBBFA0-4896-4F89-83F2-9B6F36081FF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{606D9982-FF33-4FCF-965C-160E67E8EBF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3642,6 +3781,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5DBBFA0-4896-4F89-83F2-9B6F36081FF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
New technique from ATT&CK v12 added for DeTT&CT data source
</commit_message>
<xml_diff>
--- a/data/dettect_data_sources.xlsx
+++ b/data/dettect_data_sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruben/vscode-projects/vscode-prd/DeTTECT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E223523B-8D99-4D41-97FE-3F3AF3AD579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DBCEBE-4505-704F-A36D-0C532858C190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="39880" windowHeight="25100" xr2:uid="{CA121E54-A6AA-1848-A706-0DCFA18BBC16}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="DeTT&amp;CT data sources" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Techniques!$A$1:$H$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Techniques!$A$1:$H$105</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="236">
   <si>
     <t>T1612</t>
   </si>
@@ -740,6 +740,12 @@
   </si>
   <si>
     <t>ATT&amp;CK v12 - Network Traffic Content</t>
+  </si>
+  <si>
+    <t>T1567.003</t>
+  </si>
+  <si>
+    <t>Exfiltration to Text Storage Sites</t>
   </si>
 </sst>
 </file>
@@ -802,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -810,13 +816,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -826,16 +829,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1166,13 +1159,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1180,34 +1173,34 @@
     <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="4" customWidth="1"/>
     <col min="5" max="8" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1218,22 +1211,21 @@
       <c r="B2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="C2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1242,22 +1234,21 @@
       <c r="B3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="C3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1266,22 +1257,21 @@
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="C4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1290,22 +1280,21 @@
       <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="C5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1314,18 +1303,15 @@
       <c r="B6" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="C6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1334,18 +1320,15 @@
       <c r="B7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="C7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -1354,18 +1337,15 @@
       <c r="B8" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="C8" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -1374,18 +1354,15 @@
       <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="C9" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1394,22 +1371,22 @@
       <c r="B10" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="C10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="1" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1420,18 +1397,15 @@
       <c r="B11" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="D11" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -1443,10 +1417,10 @@
       <c r="C12" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1457,22 +1431,21 @@
       <c r="B13" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="C13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1481,22 +1454,22 @@
       <c r="B14" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="C14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1507,20 +1480,18 @@
       <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="C15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1529,20 +1500,18 @@
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="C16" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1551,22 +1520,22 @@
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F17" s="9" t="s">
+      <c r="C17" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1577,18 +1546,15 @@
       <c r="B18" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="C18" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -1597,18 +1563,15 @@
       <c r="B19" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="C19" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -1617,22 +1580,22 @@
       <c r="B20" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F20" s="9" t="s">
+      <c r="C20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1643,18 +1606,15 @@
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="C21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -1663,18 +1623,15 @@
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="C22" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -1683,18 +1640,15 @@
       <c r="B23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E23" s="9" t="s">
+      <c r="C23" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -1703,18 +1657,15 @@
       <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E24" s="9" t="s">
+      <c r="C24" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -1726,10 +1677,10 @@
       <c r="C25" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E25" s="9" t="s">
+      <c r="D25" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1740,20 +1691,18 @@
       <c r="B26" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="C26" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -1762,18 +1711,15 @@
       <c r="B27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="C27" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
@@ -1782,18 +1728,15 @@
       <c r="B28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="C28" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -1802,20 +1745,18 @@
       <c r="B29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="C29" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -1824,18 +1765,15 @@
       <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="C30" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -1844,18 +1782,15 @@
       <c r="B31" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
+      <c r="C31" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -1864,18 +1799,15 @@
       <c r="B32" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+      <c r="C32" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
@@ -1884,18 +1816,15 @@
       <c r="B33" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
+      <c r="C33" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -1904,18 +1833,15 @@
       <c r="B34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
+      <c r="C34" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -1924,18 +1850,15 @@
       <c r="B35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="C35" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -1944,22 +1867,21 @@
       <c r="B36" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G36" s="9" t="s">
+      <c r="C36" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -1968,22 +1890,22 @@
       <c r="B37" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F37" s="9" t="s">
+      <c r="C37" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H37" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -1994,22 +1916,22 @@
       <c r="B38" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F38" s="9" t="s">
+      <c r="C38" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2020,22 +1942,22 @@
       <c r="B39" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F39" s="9" t="s">
+      <c r="C39" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="H39" s="1" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2049,10 +1971,10 @@
       <c r="C40" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E40" s="9" t="s">
+      <c r="D40" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>179</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -2066,20 +1988,18 @@
       <c r="B41" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="C41" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
@@ -2088,18 +2008,15 @@
       <c r="B42" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="C42" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
@@ -2108,37 +2025,32 @@
       <c r="B43" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="C43" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="1" t="s">
         <v>227</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="D44" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
@@ -2147,16 +2059,13 @@
       <c r="B45" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="4" t="s">
+      <c r="C45" s="2"/>
+      <c r="D45" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" t="s">
         <v>187</v>
       </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
@@ -2165,22 +2074,21 @@
       <c r="B46" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F46" s="9" t="s">
+      <c r="C46" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
@@ -2189,22 +2097,21 @@
       <c r="B47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F47" s="9" t="s">
+      <c r="C47" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
@@ -2213,102 +2120,88 @@
       <c r="B48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-    </row>
-    <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C48" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-    </row>
-    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C49" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-    </row>
-    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C50" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C51" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-    </row>
-    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C51" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-    </row>
-    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>224</v>
       </c>
@@ -2318,234 +2211,201 @@
       <c r="C53" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="D53" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-    </row>
-    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C54" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-    </row>
-    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C55" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-    </row>
-    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-    </row>
-    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C57" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-    </row>
-    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C58" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-    </row>
-    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C59" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C60" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-    </row>
-    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C60" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-    </row>
-    <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C61" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-    </row>
-    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C62" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-    </row>
-    <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E64" s="9" t="s">
+      <c r="C64" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-    </row>
-    <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>222</v>
       </c>
@@ -2555,949 +2415,846 @@
       <c r="C65" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+      <c r="D65" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-    </row>
-    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+      <c r="D66" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-    </row>
-    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="D67" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-    </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C68" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C69" s="12" t="s">
+      <c r="C69" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D69" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-    </row>
-    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="D69" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C70" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-    </row>
-    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C70" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C71" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-    </row>
-    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-    </row>
-    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C72" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C73" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-    </row>
-    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C74" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-    </row>
-    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C74" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F75" s="9" t="s">
+      <c r="C75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-    </row>
-    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C76" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E76" s="9" t="s">
+      <c r="C76" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E77" s="9" t="s">
+      <c r="C77" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F77" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-    </row>
-    <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="F77" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C78" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F78" s="9"/>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-    </row>
-    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C78" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C79" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-    </row>
-    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C79" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C80" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-    </row>
-    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C80" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C81" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-    </row>
-    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="C81" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C82" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E82" s="9" t="s">
+      <c r="C83" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F82" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="H82" s="9"/>
-    </row>
-    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+      <c r="F83" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="4" t="s">
+      <c r="C84" s="2"/>
+      <c r="D84" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="E84" t="s">
         <v>188</v>
       </c>
-      <c r="F83" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
-    </row>
-    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="F84" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C84" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E84" s="9" t="s">
+      <c r="C85" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-    </row>
-    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+    </row>
+    <row r="86" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C85" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
-    </row>
-    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
+      <c r="C86" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C86" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G86" s="9" t="s">
+      <c r="C87" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H86" s="9"/>
-    </row>
-    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
+    </row>
+    <row r="88" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C87" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F87" s="9" t="s">
+      <c r="C88" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G87" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H87" s="9"/>
-    </row>
-    <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
+      <c r="G88" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C88" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
-    </row>
-    <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
+      <c r="C89" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C89" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G89" s="9"/>
-      <c r="H89" s="9"/>
-    </row>
-    <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
+      <c r="C90" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C90" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G90" s="9"/>
-      <c r="H90" s="9"/>
-    </row>
-    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
+      <c r="C91" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C91" s="12" t="s">
+      <c r="C92" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D91" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F91" s="9"/>
-      <c r="G91" s="9"/>
-      <c r="H91" s="9"/>
-    </row>
-    <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+      <c r="D92" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C92" s="12" t="s">
+      <c r="C93" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-    </row>
-    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+      <c r="D93" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B94" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C93" s="12" t="s">
+      <c r="C94" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-    </row>
-    <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+      <c r="D94" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B95" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C94" s="12" t="s">
+      <c r="C95" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F94" s="9"/>
-      <c r="G94" s="9"/>
-      <c r="H94" s="9"/>
-    </row>
-    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+      <c r="D95" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C95" s="12" t="s">
+      <c r="C96" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F95" s="9" t="s">
+      <c r="D96" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G95" s="9"/>
-      <c r="H95" s="9"/>
-    </row>
-    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+    </row>
+    <row r="97" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="C97" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D96" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F96" s="9"/>
-      <c r="G96" s="9"/>
-      <c r="H96" s="9"/>
-    </row>
-    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
+      <c r="D97" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C97" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F97" s="9"/>
-      <c r="G97" s="9"/>
-      <c r="H97" s="9"/>
-    </row>
-    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
+      <c r="C98" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C98" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
-    </row>
-    <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
+      <c r="C99" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C99" s="12" t="s">
+      <c r="C100" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D99" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-    </row>
-    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
+      <c r="D100" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F100" s="9" t="s">
+      <c r="C101" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-    </row>
-    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
+    </row>
+    <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C101" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
-    </row>
-    <row r="102" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
+      <c r="C102" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C102" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E102" s="9" t="s">
+      <c r="C103" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
-    </row>
-    <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
+    </row>
+    <row r="104" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B104" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C103" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E103" s="9" t="s">
+      <c r="C104" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E104" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F103" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G103" s="9"/>
-      <c r="H103" s="9"/>
-    </row>
-    <row r="104" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
+      <c r="F104" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C104" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-    </row>
-    <row r="105" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
+      <c r="C105" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
-      <c r="H105" s="9"/>
-    </row>
-    <row r="106" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
+      <c r="C106" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F106" s="9"/>
-      <c r="G106" s="9"/>
-      <c r="H106" s="9"/>
-    </row>
-    <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
+      <c r="C107" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C107" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F107" s="9"/>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-    </row>
-    <row r="108" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
+      <c r="C108" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F108" s="9"/>
-      <c r="G108" s="9"/>
-      <c r="H108" s="9"/>
-    </row>
-    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="2" t="s">
+      <c r="C109" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C109" s="12" t="s">
+      <c r="C110" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="F109" s="9"/>
-      <c r="G109" s="9"/>
-      <c r="H109" s="9"/>
-    </row>
-    <row r="110" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
+      <c r="D110" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C110" s="12" t="s">
+      <c r="C111" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D110" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="F110" s="9"/>
-      <c r="G110" s="9"/>
-      <c r="H110" s="9"/>
+      <c r="D111" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H104" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H110">
-      <sortCondition ref="A1:A110"/>
+  <autoFilter ref="A1:H105" xr:uid="{39E03B4C-688D-3244-BF0E-1F004D35DAE6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H111">
+      <sortCondition ref="A1:A111"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H98">
-    <sortCondition ref="A1:A98"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H99">
+    <sortCondition ref="A1:A99"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -3563,6 +3320,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C10F0625C0942243B06F014CA94A1AFE" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2042c6bc1cae45920cbe57d817eddad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c6cd37b1-e58f-4b4d-9972-86df42eb1d84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="012bfb64603ca90dd9e4209826fe8536" ns2:_="">
     <xsd:import namespace="c6cd37b1-e58f-4b4d-9972-86df42eb1d84"/>
@@ -3752,22 +3524,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13F9E60B-A72D-4D36-A6ED-88D80BD28E6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c6cd37b1-e58f-4b4d-9972-86df42eb1d84"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5DBBFA0-4896-4F89-83F2-9B6F36081FF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{606D9982-FF33-4FCF-965C-160E67E8EBF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3783,28 +3564,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5DBBFA0-4896-4F89-83F2-9B6F36081FF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13F9E60B-A72D-4D36-A6ED-88D80BD28E6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c6cd37b1-e58f-4b4d-9972-86df42eb1d84"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>